<commit_message>
commit khoa hoc ki thuat
</commit_message>
<xml_diff>
--- a/TraiNghiemSangTao/TraiNghiemSangTao/Utils/Files/ds-khoahockythuat.xlsx
+++ b/TraiNghiemSangTao/TraiNghiemSangTao/Utils/Files/ds-khoahockythuat.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>DANH SÁCH ĐĂNG KÍ KHOA HỌC KỸ THUẬT</t>
   </si>
@@ -35,6 +35,9 @@
     <t>NGÀY</t>
   </si>
   <si>
+    <t>THÁNG</t>
+  </si>
+  <si>
     <t>NĂM</t>
   </si>
   <si>
@@ -50,9 +53,6 @@
     <t>TÊN HỌC SINH 2</t>
   </si>
   <si>
-    <t>THÁNG</t>
-  </si>
-  <si>
     <t>GVHD</t>
   </si>
   <si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>EMAIL</t>
+  </si>
+  <si>
+    <t>FILE</t>
   </si>
   <si>
     <t>Khoa học động vật (1)</t>
@@ -251,6 +254,9 @@
     <t>39</t>
   </si>
   <si>
+    <t>testfileupload.docx</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kỹ thuật Y Sinh (5)
 </t>
   </si>
@@ -258,12 +264,18 @@
     <t>truo huu thanh</t>
   </si>
   <si>
+    <t>data.xlsx</t>
+  </si>
+  <si>
     <t>ww adaw adw</t>
   </si>
   <si>
     <t>wea dwadwa</t>
   </si>
   <si>
+    <t>7-16</t>
+  </si>
+  <si>
     <t>wa wadawd wa</t>
   </si>
   <si>
@@ -276,6 +288,9 @@
     <t>dwad wada</t>
   </si>
   <si>
+    <t>5-17.docx</t>
+  </si>
+  <si>
     <t>dwa dwada</t>
   </si>
   <si>
@@ -286,6 +301,15 @@
   </si>
   <si>
     <t>truonghuuthanh95@gmail.com</t>
+  </si>
+  <si>
+    <t>1-18.xlsx</t>
+  </si>
+  <si>
+    <t>nguyen ha nguyen</t>
+  </si>
+  <si>
+    <t>1-19.pdf</t>
   </si>
 </sst>
 </file>
@@ -361,7 +385,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:U23"/>
+  <dimension ref="A2:V24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -483,36 +507,38 @@
       <c r="G6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="3"/>
+      <c r="H6" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="I6" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S6" s="3" t="s">
         <v>13</v>
@@ -522,6 +548,9 @@
       </c>
       <c r="U6" s="3" t="s">
         <v>15</v>
+      </c>
+      <c r="V6" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7">
@@ -529,34 +558,34 @@
         <v>1</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8">
@@ -564,55 +593,55 @@
         <v>2</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="L8" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="M8" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="N8" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="O8" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="P8" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="Q8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
@@ -620,55 +649,55 @@
         <v>3</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="M9" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="0" t="s">
+      <c r="N9" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="P9" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K9" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="M9" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="N9" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="O9" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="P9" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="Q9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="R9" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
@@ -676,55 +705,55 @@
         <v>4</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="P10" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="L10" s="0" t="s">
+      <c r="Q10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="R10" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="M10" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="N10" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="O10" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="P10" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q10" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="R10" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -732,58 +761,58 @@
         <v>5</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="G11" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="H11" s="0" t="s">
+      <c r="L11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="0" t="s">
+      <c r="O11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="P11" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K11" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="L11" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="N11" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="O11" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="P11" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="Q11" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="R11" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S11" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12">
@@ -791,58 +820,58 @@
         <v>6</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J12" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="O12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="P12" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K12" s="0" t="s">
+      <c r="Q12" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="R12" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="S12" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="L12" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="M12" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="N12" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="O12" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="P12" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q12" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="R12" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="S12" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="13">
@@ -850,37 +879,37 @@
         <v>7</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="G13" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="S13" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14">
@@ -888,58 +917,58 @@
         <v>8</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="M14" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="N14" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="O14" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="P14" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K14" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="L14" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="M14" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="N14" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="O14" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="P14" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="Q14" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="R14" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S14" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15">
@@ -947,58 +976,58 @@
         <v>9</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="K15" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="J15" s="0" t="s">
+      <c r="L15" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="M15" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="O15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="P15" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="K15" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="L15" s="0" t="s">
+      <c r="Q15" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="M15" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="N15" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="O15" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="P15" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q15" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="R15" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="S15" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16">
@@ -1006,37 +1035,37 @@
         <v>10</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="S16" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17">
@@ -1044,37 +1073,37 @@
         <v>11</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S17" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18">
@@ -1082,37 +1111,37 @@
         <v>12</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S18" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19">
@@ -1120,37 +1149,40 @@
         <v>13</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K19" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="S19" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="S19" s="0" t="s">
-        <v>76</v>
+      <c r="V19" s="0" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="20">
@@ -1158,37 +1190,40 @@
         <v>14</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S20" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
+      </c>
+      <c r="V20" s="0" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="21">
@@ -1196,37 +1231,40 @@
         <v>15</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S21" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
+      </c>
+      <c r="V21" s="0" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="22">
@@ -1234,37 +1272,40 @@
         <v>16</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S22" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
+      </c>
+      <c r="V22" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="23">
@@ -1272,64 +1313,114 @@
         <v>17</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H23" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="L23" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="M23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N23" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="O23" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="P23" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q23" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="R23" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="S23" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="T23" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="U23" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="V23" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0">
+        <v>18</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="I23" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="J23" s="0" t="s">
+      <c r="F24" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="I24" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="K23" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="L23" s="0" t="s">
+      <c r="J24" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="K24" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="S24" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="M23" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="N23" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="O23" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="P23" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q23" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="R23" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="S23" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="T23" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="U23" s="0" t="s">
-        <v>89</v>
+      <c r="T24" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="U24" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="V24" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>